<commit_message>
Knowledge base correction and paper update
</commit_message>
<xml_diff>
--- a/knowledge/autos2-knowledge_2023_04_06.xlsx
+++ b/knowledge/autos2-knowledge_2023_04_06.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CVE-ICS_ATT&amp;CK-Mapping" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="254">
   <si>
     <t>CVE ID</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Exploitation of Remote Services</t>
-  </si>
-  <si>
-    <t>Man in the Middle</t>
   </si>
   <si>
     <t>Data from Information Repositories</t>
@@ -786,7 +783,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -872,7 +869,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1160,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>50</v>
@@ -1425,7 +1422,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>34</v>
@@ -1448,7 +1445,7 @@
         <v>55</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>38</v>
@@ -1528,7 +1525,7 @@
         <v>56</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>38</v>
@@ -1609,10 +1606,10 @@
         <v>35</v>
       </c>
       <c r="E22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1620,10 +1617,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C23" t="s">
         <v>248</v>
-      </c>
-      <c r="C23" t="s">
-        <v>249</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>35</v>
@@ -1635,7 +1632,7 @@
         <v>33</v>
       </c>
       <c r="G23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,13 +1640,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>50</v>
@@ -1658,7 +1655,7 @@
         <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1666,10 +1663,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>56</v>
@@ -1681,7 +1678,7 @@
         <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1689,10 +1686,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>55</v>
@@ -1704,7 +1701,7 @@
         <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,10 +1709,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>55</v>
@@ -1727,7 +1724,7 @@
         <v>38</v>
       </c>
       <c r="G27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1841,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2066,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>45</v>
@@ -2083,7 +2080,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>44</v>
@@ -2097,7 +2094,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>45</v>
@@ -2111,7 +2108,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>45</v>
@@ -2121,12 +2118,32 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -2147,13 +2164,15 @@
     <hyperlink ref="B13" r:id="rId12"/>
     <hyperlink ref="B14" r:id="rId13"/>
     <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B16" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -2162,7 +2181,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,842 +2196,842 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="F4" t="s">
         <v>82</v>
-      </c>
-      <c r="F4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>87</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
         <v>89</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="F6" t="s">
         <v>91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
         <v>93</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" t="s">
         <v>95</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>96</v>
-      </c>
-      <c r="E7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
         <v>98</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" t="s">
         <v>100</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>101</v>
-      </c>
-      <c r="E8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
         <v>103</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" t="s">
         <v>105</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>106</v>
-      </c>
-      <c r="E9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
         <v>108</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>111</v>
-      </c>
-      <c r="E10" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
         <v>113</v>
       </c>
-      <c r="B11" t="s">
-        <v>114</v>
-      </c>
       <c r="C11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" t="s">
         <v>100</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>101</v>
-      </c>
-      <c r="E11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
         <v>115</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" t="s">
         <v>117</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>118</v>
-      </c>
-      <c r="E12" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
         <v>120</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" t="s">
         <v>122</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>123</v>
-      </c>
-      <c r="E13" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" t="s">
         <v>127</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>128</v>
-      </c>
-      <c r="E14" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s">
         <v>130</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" t="s">
         <v>132</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>133</v>
-      </c>
-      <c r="E15" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
         <v>135</v>
       </c>
-      <c r="B16" t="s">
-        <v>136</v>
-      </c>
       <c r="C16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" t="s">
         <v>127</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>128</v>
-      </c>
-      <c r="E16" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
         <v>137</v>
       </c>
-      <c r="B17" t="s">
-        <v>138</v>
-      </c>
       <c r="C17" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" t="s">
         <v>127</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>128</v>
-      </c>
-      <c r="E17" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
         <v>139</v>
       </c>
-      <c r="B18" t="s">
-        <v>140</v>
-      </c>
       <c r="C18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
         <v>86</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>87</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" t="s">
         <v>141</v>
       </c>
-      <c r="B19" t="s">
-        <v>142</v>
-      </c>
       <c r="C19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
         <v>86</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>87</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
         <v>143</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" t="s">
         <v>145</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>146</v>
-      </c>
-      <c r="E20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
         <v>148</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" t="s">
         <v>150</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>151</v>
-      </c>
-      <c r="E21" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" t="s">
-        <v>154</v>
-      </c>
       <c r="C22" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" t="s">
         <v>145</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>146</v>
-      </c>
-      <c r="E22" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" t="s">
         <v>155</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
         <v>156</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" t="s">
-        <v>157</v>
-      </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" t="s">
         <v>158</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="F24" t="s">
         <v>160</v>
-      </c>
-      <c r="F24" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" t="s">
         <v>162</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" t="s">
         <v>164</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>165</v>
-      </c>
-      <c r="E25" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" t="s">
         <v>167</v>
-      </c>
-      <c r="B26" t="s">
-        <v>168</v>
       </c>
       <c r="C26" s="7"/>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" t="s">
         <v>170</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" t="s">
         <v>172</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>173</v>
-      </c>
-      <c r="E27" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
         <v>175</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" t="s">
         <v>176</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F28" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" t="s">
         <v>178</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" t="s">
         <v>180</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>181</v>
-      </c>
-      <c r="E29" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" t="s">
         <v>183</v>
       </c>
-      <c r="B30" t="s">
-        <v>184</v>
-      </c>
       <c r="C30" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" t="s">
         <v>145</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>146</v>
-      </c>
-      <c r="E30" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" t="s">
         <v>185</v>
       </c>
-      <c r="B31" t="s">
-        <v>186</v>
-      </c>
       <c r="C31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" t="s">
         <v>132</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>133</v>
-      </c>
-      <c r="E31" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" t="s">
         <v>187</v>
       </c>
-      <c r="B32" t="s">
-        <v>188</v>
-      </c>
       <c r="C32" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s">
         <v>127</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>128</v>
-      </c>
-      <c r="E32" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" t="s">
         <v>189</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="F33" t="s">
         <v>191</v>
-      </c>
-      <c r="F33" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
         <v>193</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" t="s">
         <v>195</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>196</v>
-      </c>
-      <c r="E34" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" t="s">
         <v>198</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
         <v>199</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>200</v>
-      </c>
-      <c r="E35" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="s">
         <v>202</v>
       </c>
-      <c r="B36" t="s">
-        <v>203</v>
-      </c>
       <c r="C36" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" t="s">
         <v>191</v>
-      </c>
-      <c r="F36" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" t="s">
         <v>204</v>
       </c>
-      <c r="B37" t="s">
-        <v>205</v>
-      </c>
       <c r="C37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
         <v>105</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>106</v>
-      </c>
-      <c r="E37" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38" t="s">
         <v>206</v>
       </c>
-      <c r="B38" t="s">
-        <v>207</v>
-      </c>
       <c r="C38" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" t="s">
         <v>132</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>133</v>
-      </c>
-      <c r="E38" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
         <v>208</v>
       </c>
-      <c r="B39" t="s">
-        <v>209</v>
-      </c>
       <c r="C39" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" t="s">
         <v>105</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>106</v>
-      </c>
-      <c r="E39" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>209</v>
+      </c>
+      <c r="B40" t="s">
         <v>210</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" t="s">
         <v>212</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>213</v>
-      </c>
-      <c r="E40" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>214</v>
+      </c>
+      <c r="B41" t="s">
         <v>215</v>
       </c>
-      <c r="B41" t="s">
-        <v>216</v>
-      </c>
       <c r="C41" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" t="s">
         <v>217</v>
       </c>
-      <c r="B42" t="s">
-        <v>218</v>
-      </c>
       <c r="C42" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" t="s">
         <v>132</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>133</v>
-      </c>
-      <c r="E42" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" t="s">
         <v>219</v>
       </c>
-      <c r="B43" t="s">
-        <v>220</v>
-      </c>
       <c r="C43" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
         <v>72</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>73</v>
-      </c>
-      <c r="E43" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>220</v>
+      </c>
+      <c r="B44" t="s">
         <v>221</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F44" t="s">
         <v>222</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F44" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>223</v>
+      </c>
+      <c r="B45" t="s">
         <v>224</v>
       </c>
-      <c r="B45" t="s">
-        <v>225</v>
-      </c>
       <c r="C45" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" t="s">
         <v>132</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>133</v>
-      </c>
-      <c r="E45" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B46" t="s">
         <v>226</v>
-      </c>
-      <c r="B46" t="s">
-        <v>227</v>
       </c>
       <c r="C46" s="7"/>
       <c r="F46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>228</v>
+      </c>
+      <c r="B47" t="s">
         <v>229</v>
-      </c>
-      <c r="B47" t="s">
-        <v>230</v>
       </c>
       <c r="C47" s="7"/>
       <c r="F47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>230</v>
+      </c>
+      <c r="B48" t="s">
         <v>231</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="D48" t="s">
         <v>233</v>
       </c>
-      <c r="D48" t="s">
-        <v>234</v>
-      </c>
       <c r="E48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>234</v>
+      </c>
+      <c r="B49" t="s">
         <v>235</v>
       </c>
-      <c r="B49" t="s">
-        <v>236</v>
-      </c>
       <c r="C49" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
+        <v>199</v>
+      </c>
+      <c r="E49" t="s">
         <v>200</v>
-      </c>
-      <c r="E49" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>236</v>
+      </c>
+      <c r="B50" t="s">
         <v>237</v>
-      </c>
-      <c r="B50" t="s">
-        <v>238</v>
       </c>
       <c r="C50" s="7"/>
       <c r="F50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>239</v>
+      </c>
+      <c r="B51" t="s">
         <v>240</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="F51" t="s">
         <v>242</v>
-      </c>
-      <c r="F51" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" t="s">
         <v>244</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="D52" t="s">
         <v>246</v>
       </c>
-      <c r="D52" t="s">
-        <v>247</v>
-      </c>
       <c r="E52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>